<commit_message>
feat(testcase) : add new function
Description :
新增判断：ID号为空、ID号重复报错
ID号加入excel表中，用例名称后面的序号
excel表中用例名称的序号，转成xmind的时候，在步骤中加上

Change-Id: Ia849875035bf52644a3ba8bd8664699db78418d9
</commit_message>
<xml_diff>
--- a/src/automotive/application/testcase/writer/template_sample.xlsx
+++ b/src/automotive/application/testcase/writer/template_sample.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Chinatsp\develop\python\src\automotive\application\testcase\writer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\automotive_rel\automotive\src\automotive\application\testcase\writer\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDD2010-8145-4D8E-BEDD-4755E486CE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13650" yWindow="7845" windowWidth="13905" windowHeight="14070" activeTab="1"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>测试数据统计</t>
   </si>
@@ -111,13 +112,17 @@
   </si>
   <si>
     <t>测试结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改记录</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -204,7 +209,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -279,13 +284,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -307,6 +349,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -344,6 +389,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -625,57 +679,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="10"/>
     </row>
-    <row r="2" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14" t="s">
+      <c r="F2" s="14"/>
+      <c r="G2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="16" t="s">
+      <c r="H2" s="16"/>
+      <c r="I2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="17"/>
+      <c r="J2" s="18"/>
       <c r="K2" s="2" t="s">
         <v>7</v>
       </c>
@@ -707,43 +761,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="26.25" customWidth="1"/>
-    <col min="4" max="7" width="35.625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="26.21875" customWidth="1"/>
+    <col min="4" max="7" width="35.6640625" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5" customWidth="1"/>
+    <col min="13" max="13" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="19" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
     </row>
-    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -771,26 +826,29 @@
       <c r="I2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>